<commit_message>
updated to version 0.0.5
</commit_message>
<xml_diff>
--- a/SASPACer/addcnt/template_package.xlsx
+++ b/SASPACer/addcnt/template_package.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mytakeda-my.sharepoint.com/personal/ryou_nakaya_takeda_com/Documents/仲家/SAS/SASPACer/SASPACer/addcnt/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="245" documentId="11_F25DC773A252ABDACC104856C95E563E5ADE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2FF3A541-5333-4330-8091-9D16FCD898BB}"/>
+  <xr:revisionPtr revIDLastSave="248" documentId="11_F25DC773A252ABDACC104856C95E563E5ADE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E3C921ED-DDFB-4996-96EE-92784006ED5E}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" tabRatio="863" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4020" yWindow="3140" windowWidth="14400" windowHeight="8260" tabRatio="863" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="description" sheetId="1" r:id="rId1"/>
@@ -1434,16 +1434,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2407937D-6862-4C42-A8B5-594F375883D2}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" customWidth="1"/>
-    <col min="2" max="2" width="40.9140625" style="1" customWidth="1"/>
-    <col min="3" max="4" width="36.9140625" customWidth="1"/>
+    <col min="1" max="1" width="11.08203125" customWidth="1"/>
+    <col min="2" max="2" width="24.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="36.9140625" customWidth="1"/>
+    <col min="4" max="4" width="23.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1536,7 +1537,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F138A73F-DE48-4877-AA04-F53F95AC3500}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>

</xml_diff>